<commit_message>
Refactor bench.py to include parallel versions of hill-climbing and simulated-annealing algorithms
</commit_message>
<xml_diff>
--- a/Trabajo/Data/test/diferenciaCPU2-1.xlsx
+++ b/Trabajo/Data/test/diferenciaCPU2-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ketbome\Desktop\Projects\Electivo\Trabajo\Data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F319E7-09A8-46C8-A9C7-B613037BBA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502ED45-B996-4D48-8AFF-55A7F7F537F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiempos" sheetId="1" r:id="rId1"/>
@@ -574,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
@@ -856,11 +856,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>